<commit_message>
Data file and Registration test case added
</commit_message>
<xml_diff>
--- a/DataOne-Registration.Sami.xlsx
+++ b/DataOne-Registration.Sami.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rashids2\Documents\GitHub\CBIITQA-ICRC-KICKOFF\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kaurs3\Documents\GitHub\CBIITQA-ICRC-KICKOFF\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{400E1B7F-7723-4ACD-B860-9C2E1CDD14EA}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{256C9F8D-81CA-4CDA-81FD-967D8F319735}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23016" windowHeight="9048" activeTab="1" xr2:uid="{8B883429-13CF-4D4F-8813-CE891B7D6AFB}"/>
   </bookViews>
@@ -76,19 +76,19 @@
     <t>LastName12</t>
   </si>
   <si>
-    <t>ncitester11@nih.gov</t>
-  </si>
-  <si>
-    <t>ncitester12@nih.gov</t>
-  </si>
-  <si>
     <t>FirstName13</t>
   </si>
   <si>
     <t>LastName13</t>
   </si>
   <si>
-    <t>ncitester13@nih.gov</t>
+    <t>ncitester15@nih.gov</t>
+  </si>
+  <si>
+    <t>ncitester16@nih.gov</t>
+  </si>
+  <si>
+    <t>ncitester17@nih.gov</t>
   </si>
 </sst>
 </file>
@@ -535,7 +535,7 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -565,7 +565,7 @@
         <v>13</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D2" s="3"/>
       <c r="E2" s="3"/>
@@ -578,17 +578,17 @@
         <v>15</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D3" s="3"/>
       <c r="E3" s="3"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>20</v>

</xml_diff>